<commit_message>
double checks and updates metadata
</commit_message>
<xml_diff>
--- a/data-raw/metadata/lower_feather_catch_metadata.xlsx
+++ b/data-raw/metadata/lower_feather_catch_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badhia\Documents\git\jpe-lower-feather-edi\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F09DB5D-F03E-4A71-AC04-D89710F049F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{775CE5C5-49CA-4D17-8225-E93A928318F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4940" yWindow="2630" windowWidth="19200" windowHeight="11170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -280,7 +280,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -306,7 +306,6 @@
     <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -526,7 +525,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="L14" sqref="L14:M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1076,7 +1075,7 @@
         <v>44580.520960648151</v>
       </c>
       <c r="M13" s="10">
-        <v>45456.01090277778</v>
+        <v>45809.406828703701</v>
       </c>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
@@ -1116,8 +1115,12 @@
         <v>39</v>
       </c>
       <c r="K14" s="6"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="13"/>
+      <c r="L14" s="10">
+        <v>44580.520960648151</v>
+      </c>
+      <c r="M14" s="10">
+        <v>45809.406828703701</v>
+      </c>
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
       <c r="P14" s="4"/>

</xml_diff>

<commit_message>
updates catch table and metadata to have trap start and end date, and actual count
</commit_message>
<xml_diff>
--- a/data-raw/metadata/lower_feather_catch_metadata.xlsx
+++ b/data-raw/metadata/lower_feather_catch_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badhia\Documents\git\jpe-lower-feather-edi\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{775CE5C5-49CA-4D17-8225-E93A928318F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F781F291-20E6-45C4-8279-E31A9138ABE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1300" yWindow="680" windowWidth="17670" windowHeight="13710" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="70">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -219,6 +219,24 @@
   </si>
   <si>
     <t xml:space="preserve">Date and time of day associated with the end of trap visit. Definition varies based on visitType. </t>
+  </si>
+  <si>
+    <t>trap_start_date</t>
+  </si>
+  <si>
+    <t>Start date and time of a trapping period. Derived from visitTime and visitTime2 fields, adjusted based on the visitType field</t>
+  </si>
+  <si>
+    <t>trap_end_date</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> End date and time of a trapping period. Derived from visitTime and visitTime2 fields, adjusted based on the visitType field</t>
+  </si>
+  <si>
+    <t>actualCount</t>
+  </si>
+  <si>
+    <t>Whether the count (n) is an actual count or estimate. Levels = c("Yes", "No")</t>
   </si>
 </sst>
 </file>
@@ -521,11 +539,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z998"/>
+  <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L14" sqref="L14:M14"/>
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1288,11 +1306,21 @@
       <c r="Z18" s="1"/>
     </row>
     <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="4"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="1"/>
+      <c r="A19" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
@@ -1316,19 +1344,35 @@
       <c r="Z19" s="1"/>
     </row>
     <row r="20" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="4"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="6"/>
-      <c r="L20" s="10"/>
-      <c r="M20" s="10"/>
+      <c r="A20" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="K20" s="2"/>
+      <c r="L20" s="10">
+        <v>44580.520960648151</v>
+      </c>
+      <c r="M20" s="10">
+        <v>45809.406828703701</v>
+      </c>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
@@ -1344,19 +1388,35 @@
       <c r="Z20" s="1"/>
     </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="4"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="1"/>
+      <c r="A21" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
       <c r="I21" s="6"/>
-      <c r="J21" s="5"/>
+      <c r="J21" s="5" t="s">
+        <v>39</v>
+      </c>
       <c r="K21" s="6"/>
-      <c r="L21" s="5"/>
-      <c r="M21" s="5"/>
+      <c r="L21" s="10">
+        <v>44580.520960648151</v>
+      </c>
+      <c r="M21" s="10">
+        <v>45809.406828703701</v>
+      </c>
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
@@ -1377,14 +1437,14 @@
       <c r="C22" s="1"/>
       <c r="D22" s="2"/>
       <c r="E22" s="1"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="2"/>
-      <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
@@ -1456,6 +1516,19 @@
       <c r="Z24" s="1"/>
     </row>
     <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="4"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
@@ -1471,14 +1544,6 @@
       <c r="Z25" s="1"/>
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="3"/>
-      <c r="K26" s="2"/>
-      <c r="L26" s="3"/>
-      <c r="M26" s="3"/>
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
@@ -1494,6 +1559,14 @@
       <c r="Z26" s="1"/>
     </row>
     <row r="27" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
       <c r="N27" s="4"/>
       <c r="O27" s="4"/>
       <c r="P27" s="4"/>
@@ -1554,19 +1627,6 @@
       <c r="Z30" s="1"/>
     </row>
     <row r="31" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="4"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="3"/>
-      <c r="K31" s="2"/>
-      <c r="L31" s="3"/>
-      <c r="M31" s="3"/>
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
       <c r="P31" s="1"/>
@@ -1666,7 +1726,7 @@
       <c r="Z34" s="1"/>
     </row>
     <row r="35" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="11"/>
+      <c r="A35" s="4"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="2"/>
@@ -1694,7 +1754,7 @@
       <c r="Z35" s="1"/>
     </row>
     <row r="36" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="12"/>
+      <c r="A36" s="11"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="2"/>
@@ -1722,7 +1782,7 @@
       <c r="Z36" s="1"/>
     </row>
     <row r="37" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="11"/>
+      <c r="A37" s="12"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="2"/>
@@ -1750,7 +1810,7 @@
       <c r="Z37" s="1"/>
     </row>
     <row r="38" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="12"/>
+      <c r="A38" s="11"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="2"/>
@@ -1778,7 +1838,7 @@
       <c r="Z38" s="1"/>
     </row>
     <row r="39" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="4"/>
+      <c r="A39" s="12"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="2"/>
@@ -2730,7 +2790,7 @@
       <c r="Z72" s="1"/>
     </row>
     <row r="73" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="1"/>
+      <c r="A73" s="4"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
       <c r="D73" s="2"/>
@@ -28657,22 +28717,37 @@
       <c r="Y998" s="1"/>
       <c r="Z998" s="1"/>
     </row>
+    <row r="999" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A999" s="1"/>
+      <c r="B999" s="1"/>
+      <c r="C999" s="1"/>
+      <c r="D999" s="2"/>
+      <c r="E999" s="1"/>
+      <c r="F999" s="3"/>
+      <c r="G999" s="3"/>
+      <c r="H999" s="3"/>
+      <c r="I999" s="2"/>
+      <c r="J999" s="3"/>
+      <c r="K999" s="2"/>
+      <c r="L999" s="3"/>
+      <c r="M999" s="3"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="A38:A39"/>
   </mergeCells>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C55:C998 C31:C43 C1:C24" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C56:C999 C32:C44 C1:C25" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"nominal,ordinal,interval,ratio,dateTime"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E31:E998 E1:E24" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E32:E999 E1:E25" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"text,enumerated,dateTime,numeric"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F26 F31:F998 F1:F24" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F27 F32:F999 F1:F25" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"ratio,interval"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H26 H31:H998 H1:H24" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H27 H32:H999 H1:H25" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"natural,whole,integer,real"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
updates processed and clean data files, updates metadata
</commit_message>
<xml_diff>
--- a/data-raw/metadata/lower_feather_catch_metadata.xlsx
+++ b/data-raw/metadata/lower_feather_catch_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badhia\Documents\git\jpe-lower-feather-edi\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F781F291-20E6-45C4-8279-E31A9138ABE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F36E3571-00C5-4FC0-80F6-36F7055F0530}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1300" yWindow="680" windowWidth="17670" windowHeight="13710" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5560" yWindow="2350" windowWidth="19200" windowHeight="11170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -542,8 +542,8 @@
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1093,7 +1093,7 @@
         <v>44580.520960648151</v>
       </c>
       <c r="M13" s="10">
-        <v>45809.406828703701</v>
+        <v>46003.427627314813</v>
       </c>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
@@ -1137,7 +1137,7 @@
         <v>44580.520960648151</v>
       </c>
       <c r="M14" s="10">
-        <v>45809.406828703701</v>
+        <v>46003.427627314813</v>
       </c>
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
@@ -1371,7 +1371,7 @@
         <v>44580.520960648151</v>
       </c>
       <c r="M20" s="10">
-        <v>45809.406828703701</v>
+        <v>46003.427627314813</v>
       </c>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
@@ -1415,7 +1415,7 @@
         <v>44580.520960648151</v>
       </c>
       <c r="M21" s="10">
-        <v>45809.406828703701</v>
+        <v>46003.427627314813</v>
       </c>
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>

</xml_diff>